<commit_message>
Adicionado a classe para pesquisar produto na lupa e a classe de Sua pageobject, adicionado novo diretorio para as screenshot do novo teste.
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\Documents\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\ProjetoAvaliação\Avaliacao\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990E407F-7DBB-4D52-B0EC-40E2DA8FDF8B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D182F11C-D75E-462E-AAD0-905DB7EB65F0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="1065" windowWidth="15375" windowHeight="7875" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
+    <workbookView xWindow="4050" yWindow="3300" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Contas" sheetId="1" r:id="rId1"/>
+    <sheet name="BuscaLupa" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Matheus</t>
   </si>
@@ -69,9 +70,6 @@
     <t>Cep</t>
   </si>
   <si>
-    <t>AmimV</t>
-  </si>
-  <si>
     <t>matheus.amim@hotmail.com</t>
   </si>
   <si>
@@ -87,9 +85,6 @@
     <t>Emilio Lehmann,120</t>
   </si>
   <si>
-    <t>SP</t>
-  </si>
-  <si>
     <t>06695-480</t>
   </si>
   <si>
@@ -124,6 +119,21 @@
   </si>
   <si>
     <t>Brazil</t>
+  </si>
+  <si>
+    <t>sadsxzu</t>
+  </si>
+  <si>
+    <t>Spdasdasds</t>
+  </si>
+  <si>
+    <t>HeadSet</t>
+  </si>
+  <si>
+    <t>/html/body/div[3]/section/article/div[3]/div/div/div[2]/ul/li[2]/img</t>
+  </si>
+  <si>
+    <t>/html/body/div[3]/section/article/div[3]/div/div/div[2]/ul/li[1]/img</t>
   </si>
 </sst>
 </file>
@@ -176,10 +186,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -497,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E93621F3-1ABA-4547-8339-842847F49F65}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +546,7 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -552,13 +563,13 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -567,54 +578,54 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
         <v>30</v>
       </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>23</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>25</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>26</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -631,4 +642,41 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A469EE5-3D0C-467A-8AB5-81E170E63C51}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="63.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Atualizado os nomes dos pacotes do projeto, atualizado os metodos para as screenshot, adicionado um try catch para retornar se o resultado foi o mesmo esperado.
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\ProjetoAvaliação\Avaliacao\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D182F11C-D75E-462E-AAD0-905DB7EB65F0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85116755-A63B-4BB9-91C5-71C4642E4868}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4050" yWindow="3300" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Contas" sheetId="1" r:id="rId1"/>
     <sheet name="BuscaLupa" sheetId="2" r:id="rId2"/>
+    <sheet name="BuscaHome" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Matheus</t>
   </si>
@@ -121,26 +122,41 @@
     <t>Brazil</t>
   </si>
   <si>
-    <t>sadsxzu</t>
-  </si>
-  <si>
     <t>Spdasdasds</t>
   </si>
   <si>
-    <t>HeadSet</t>
-  </si>
-  <si>
-    <t>/html/body/div[3]/section/article/div[3]/div/div/div[2]/ul/li[2]/img</t>
-  </si>
-  <si>
-    <t>/html/body/div[3]/section/article/div[3]/div/div/div[2]/ul/li[1]/img</t>
+    <t>Logitech USB Headset H390</t>
+  </si>
+  <si>
+    <t>LapTop</t>
+  </si>
+  <si>
+    <t>HP ENVY - 17t Touch Laptop</t>
+  </si>
+  <si>
+    <t>Headset</t>
+  </si>
+  <si>
+    <t>carro</t>
+  </si>
+  <si>
+    <t>https://www.advantageonlineshopping.com/#/product/14?viewAll=Headset</t>
+  </si>
+  <si>
+    <t>AmimVieira</t>
+  </si>
+  <si>
+    <t>Nome Produtos</t>
+  </si>
+  <si>
+    <t>HP Pro Tablet 608 G1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +180,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -186,11 +208,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -508,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E93621F3-1ABA-4547-8339-842847F49F65}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,7 +586,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
@@ -590,7 +613,7 @@
         <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K2" t="s">
         <v>17</v>
@@ -614,6 +637,9 @@
       </c>
       <c r="F3" t="s">
         <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
       </c>
       <c r="H3" t="s">
         <v>23</v>
@@ -646,34 +672,76 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A469EE5-3D0C-467A-8AB5-81E170E63C51}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" location="/product/14?viewAll=Headset" xr:uid="{57226DC9-68DE-4FEB-8AE1-E8B7866EF284}"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91637A43-323E-4909-B4CF-65559BD2B712}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A2" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Adicionado teste para a falha dos cenarios e para o print de todos os cenarios, acrescentado dados a massa de dados.
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\ProjetoAvaliação\Avaliacao\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85116755-A63B-4BB9-91C5-71C4642E4868}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51BC4AE-847E-4318-ADED-00F5962CBB11}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Contas" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Matheus</t>
   </si>
@@ -128,35 +128,32 @@
     <t>Logitech USB Headset H390</t>
   </si>
   <si>
-    <t>LapTop</t>
-  </si>
-  <si>
-    <t>HP ENVY - 17t Touch Laptop</t>
-  </si>
-  <si>
     <t>Headset</t>
   </si>
   <si>
-    <t>carro</t>
-  </si>
-  <si>
     <t>https://www.advantageonlineshopping.com/#/product/14?viewAll=Headset</t>
   </si>
   <si>
-    <t>AmimVieira</t>
-  </si>
-  <si>
-    <t>Nome Produtos</t>
-  </si>
-  <si>
     <t>HP Pro Tablet 608 G1</t>
+  </si>
+  <si>
+    <t>https://www.advantageonlineshopping.com/#/product/18</t>
+  </si>
+  <si>
+    <t>Tenis</t>
+  </si>
+  <si>
+    <t>https://www.advantageonlineshopping.com/#/</t>
+  </si>
+  <si>
+    <t>MatheusVieira</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,12 +177,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF222222"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -208,12 +199,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -529,9 +519,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E93621F3-1ABA-4547-8339-842847F49F65}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -546,10 +536,11 @@
     <col min="8" max="8" width="10.28515625" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" customWidth="1"/>
+    <col min="12" max="12" width="44.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -584,9 +575,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
@@ -618,8 +609,11 @@
       <c r="K2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -654,28 +648,32 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I5" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F8" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{D868038A-3265-4776-B616-35A1FE857EEF}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{348E6C8F-65C8-4DD2-BED7-A02BB8BDB3DD}"/>
+    <hyperlink ref="L2" r:id="rId3" location="/" xr:uid="{083D1978-5373-4F74-9160-DA28F87CBAF0}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A469EE5-3D0C-467A-8AB5-81E170E63C51}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,31 +682,25 @@
     <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
     </row>
   </sheetData>
@@ -722,29 +714,38 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91637A43-323E-4909-B4CF-65559BD2B712}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" location="/product/14?viewAll=Headset" xr:uid="{DD3FEDCC-69AA-494C-B1A6-5EF810340F4E}"/>
+    <hyperlink ref="A2" r:id="rId2" location="/product/18" xr:uid="{ECC5840A-7675-4CEF-AFF7-5330259503F9}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adicionado o TestNG no projeto, e atualizado para que os teste de sucesso e falha seja executado junto
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\ProjetoAvaliação\Avaliacao\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51BC4AE-847E-4318-ADED-00F5962CBB11}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211E6AD9-AF6A-40E8-94C3-8A65F6CC93BD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Matheus</t>
   </si>
@@ -146,7 +146,10 @@
     <t>https://www.advantageonlineshopping.com/#/</t>
   </si>
   <si>
-    <t>MatheusVieira</t>
+    <t>https://www.advantageonlineshopping.com/#/category/Tablets/3</t>
+  </si>
+  <si>
+    <t>kirxhzees7</t>
   </si>
 </sst>
 </file>
@@ -577,7 +580,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
@@ -673,7 +676,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,7 +719,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91637A43-323E-4909-B4CF-65559BD2B712}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -737,12 +742,12 @@
         <v>34</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" location="/product/14?viewAll=Headset" xr:uid="{DD3FEDCC-69AA-494C-B1A6-5EF810340F4E}"/>
+    <hyperlink ref="B2" r:id="rId1" location="/category/Tablets/3" xr:uid="{DD3FEDCC-69AA-494C-B1A6-5EF810340F4E}"/>
     <hyperlink ref="A2" r:id="rId2" location="/product/18" xr:uid="{ECC5840A-7675-4CEF-AFF7-5330259503F9}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Foi adicionado as ações na mesma classe que a PageFactory, alterado o metodo de pesquisar o produto, agora não é preciso colocar o elemento na massa de dados, apenas o Nome do produto
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\ProjetoAvaliação\Avaliacao\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211E6AD9-AF6A-40E8-94C3-8A65F6CC93BD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1505443D-FD9A-4B08-8587-CCA5724510DC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Matheus</t>
   </si>
@@ -125,31 +125,22 @@
     <t>Spdasdasds</t>
   </si>
   <si>
-    <t>Logitech USB Headset H390</t>
-  </si>
-  <si>
     <t>Headset</t>
   </si>
   <si>
-    <t>https://www.advantageonlineshopping.com/#/product/14?viewAll=Headset</t>
-  </si>
-  <si>
-    <t>HP Pro Tablet 608 G1</t>
-  </si>
-  <si>
-    <t>https://www.advantageonlineshopping.com/#/product/18</t>
-  </si>
-  <si>
     <t>Tenis</t>
   </si>
   <si>
-    <t>https://www.advantageonlineshopping.com/#/</t>
-  </si>
-  <si>
-    <t>https://www.advantageonlineshopping.com/#/category/Tablets/3</t>
-  </si>
-  <si>
-    <t>kirxhzees7</t>
+    <t>Tablet 608</t>
+  </si>
+  <si>
+    <t>Headset H390</t>
+  </si>
+  <si>
+    <t>chiclete</t>
+  </si>
+  <si>
+    <t>Amidffffrd</t>
   </si>
 </sst>
 </file>
@@ -580,7 +571,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
@@ -612,9 +603,7 @@
       <c r="K2" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -664,19 +653,18 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{D868038A-3265-4776-B616-35A1FE857EEF}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{348E6C8F-65C8-4DD2-BED7-A02BB8BDB3DD}"/>
-    <hyperlink ref="L2" r:id="rId3" location="/" xr:uid="{083D1978-5373-4F74-9160-DA28F87CBAF0}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A469EE5-3D0C-467A-8AB5-81E170E63C51}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,33 +673,31 @@
     <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" location="/product/14?viewAll=Headset" xr:uid="{57226DC9-68DE-4FEB-8AE1-E8B7866EF284}"/>
-  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -731,26 +717,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" location="/category/Tablets/3" xr:uid="{DD3FEDCC-69AA-494C-B1A6-5EF810340F4E}"/>
-    <hyperlink ref="A2" r:id="rId2" location="/product/18" xr:uid="{ECC5840A-7675-4CEF-AFF7-5330259503F9}"/>
-  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adicionado uma classe que pega as celulas do Excel e passa para um metodo, assim adicionando as acoes na PageFactory sem precisar passar as celulas apenas chamando os metodos, na classe TesteCriaConta agora também esta só chamando os metodos da PageFactory e alterado os Assert's, para quando for sucesso ele capturar o nome de usuario que está logado e comparar com a celula da massa de dados que está passando o nome de usuario, no caso de false capturar o nome do erro na pagina
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\ProjetoAvaliação\Avaliacao\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1505443D-FD9A-4B08-8587-CCA5724510DC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2296484D-385B-47F1-845F-F96703447C84}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="13995" windowHeight="8025" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Contas" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Matheus</t>
   </si>
@@ -140,7 +140,10 @@
     <t>chiclete</t>
   </si>
   <si>
-    <t>Amidffffrd</t>
+    <t>Confirmar Senha</t>
+  </si>
+  <si>
+    <t>AmimGers</t>
   </si>
 </sst>
 </file>
@@ -513,7 +516,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E93621F3-1ABA-4547-8339-842847F49F65}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -522,19 +525,20 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
-    <col min="12" max="12" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
+    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" customWidth="1"/>
+    <col min="13" max="13" width="44.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -545,109 +549,118 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>28</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>29</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>22</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>28</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>23</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>24</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>25</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I5" s="2"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F8" s="2"/>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J5" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G8" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
inserido as classes de massa de dados para todos os testes, inserido o driverFactory nos teste
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\ProjetoAvaliação\Avaliacao\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2296484D-385B-47F1-845F-F96703447C84}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CDB4F2-ED3F-4625-A96C-407F032A06A8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="13995" windowHeight="8025" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
+    <workbookView xWindow="-14580" yWindow="5025" windowWidth="11520" windowHeight="7875" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Contas" sheetId="1" r:id="rId1"/>
@@ -131,9 +131,6 @@
     <t>Tenis</t>
   </si>
   <si>
-    <t>Tablet 608</t>
-  </si>
-  <si>
     <t>Headset H390</t>
   </si>
   <si>
@@ -143,7 +140,10 @@
     <t>Confirmar Senha</t>
   </si>
   <si>
-    <t>AmimGers</t>
+    <t>HP Pro</t>
+  </si>
+  <si>
+    <t>AmiViFF</t>
   </si>
 </sst>
 </file>
@@ -549,7 +549,7 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -694,12 +694,12 @@
         <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -718,9 +718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91637A43-323E-4909-B4CF-65559BD2B712}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -730,10 +728,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
         <v>32</v>
-      </c>
-      <c r="B1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Alterado o metodo de gerar o report e a screenshot gera junto ao report agora.
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\ProjetoAvaliação\Avaliacao\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CDB4F2-ED3F-4625-A96C-407F032A06A8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3836C1B-D812-481B-947F-752FF0DEEF51}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14580" yWindow="5025" windowWidth="11520" windowHeight="7875" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Contas" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
     <t>HP Pro</t>
   </si>
   <si>
-    <t>AmiViFF</t>
+    <t>Oiix65</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Refatorado o código e renomeado alguns pacotes.
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\ProjetoAvaliação\Avaliacao\target\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\Desktop\Parte\Avaliacao\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3836C1B-D812-481B-947F-752FF0DEEF51}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A8A382-E3F9-442F-BF27-FD43D428193B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
+    <workbookView xWindow="3120" yWindow="2340" windowWidth="13020" windowHeight="7875" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Contas" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
     <t>HP Pro</t>
   </si>
   <si>
-    <t>Oiix65</t>
+    <t>Oiixi6</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Alterado o metodo de assert referente ao teste de sucesso de Pesquisar produto na Lupa, alterado o caminho dos relatorios do report e deletado classe de Print Diretorio que não estava sendo mais utilizada pois as SS estão em conjunto com os reportes.
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\Desktop\Parte\Avaliacao\target\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\Desktop\MeuProjeto\Avaliacao\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A8A382-E3F9-442F-BF27-FD43D428193B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC0383C-F261-45EB-95E4-6D6172A42285}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="2340" windowWidth="13020" windowHeight="7875" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Contas" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>Matheus</t>
   </si>
@@ -134,16 +134,19 @@
     <t>Headset H390</t>
   </si>
   <si>
-    <t>chiclete</t>
-  </si>
-  <si>
     <t>Confirmar Senha</t>
   </si>
   <si>
     <t>HP Pro</t>
   </si>
   <si>
-    <t>Oiixi6</t>
+    <t>laptop</t>
+  </si>
+  <si>
+    <t>HP Stream</t>
+  </si>
+  <si>
+    <t>Miiera5</t>
   </si>
 </sst>
 </file>
@@ -549,7 +552,7 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -578,7 +581,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
@@ -677,7 +680,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,17 +691,20 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>31</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -728,7 +734,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Foi refatorado o codigo e implementado algumas boas praticas.
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\Desktop\MeuProjeto\Avaliacao\target\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\Desktop\Apresentando\Avaliacao\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC0383C-F261-45EB-95E4-6D6172A42285}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B3E6CB-B5BE-4AF0-BA94-191363AD09F4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
+    <workbookView xWindow="1860" yWindow="2205" windowWidth="15375" windowHeight="7875" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Contas" sheetId="1" r:id="rId1"/>
@@ -146,7 +146,7 @@
     <t>HP Stream</t>
   </si>
   <si>
-    <t>Miiera5</t>
+    <t>Miiera7</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Alterado a massa de dados do excel.
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\Desktop\Projeto\Avaliacao\target\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\Desktop\123\Avaliacao\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED0C414-880F-4FF2-BE9D-929819523DCB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BCE246-250A-4CE6-BB0E-059A23F72B27}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="2205" windowWidth="15375" windowHeight="7875" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
+    <workbookView xWindow="1860" yWindow="2205" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Contas" sheetId="1" r:id="rId1"/>
@@ -521,7 +521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E93621F3-1ABA-4547-8339-842847F49F65}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A469EE5-3D0C-467A-8AB5-81E170E63C51}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,10 +691,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
         <v>35</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
       </c>
       <c r="C1" t="s">
         <v>31</v>
@@ -702,10 +702,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
         <v>36</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>